<commit_message>
continuo miglioramento tuning PPO e inizio test tuning SAC
</commit_message>
<xml_diff>
--- a/Docs/Best Rewards.xlsx
+++ b/Docs/Best Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignazioemanuelepicciche/Documents/Ignazio PC/ucbm/deep_learning/Reinforcement_Learning_MuJoCu/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171F7FB6-1014-7848-9690-67997314135F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40D581A-D841-3849-A759-DD3053026B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{C9C1077D-C134-CF42-B9E2-07BC45F34DC1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="232">
   <si>
     <t xml:space="preserve"> 'n_steps': 4096</t>
   </si>
@@ -639,13 +639,106 @@
   </si>
   <si>
     <t xml:space="preserve"> 'ent_coef': 0.013922688117154487}.</t>
+  </si>
+  <si>
+    <t>{'reset_noise_scale': 0.10340640550745006</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'forward_reward_weight': 1.7316798226755399</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ctrl_cost_weight': 1.3431791463786378</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'healthy_reward': 2.4675748630080876</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'contact_cost_weight': 9.874201288446414e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'healthy_z_lower': 0.3483299533071902</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'healthy_z_upper': 1.2738868349210701</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'contact_force_min': -1.1329009828313024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'contact_force_max': 0.9421168936981189</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'learning_rate': 0.0008288719683865925</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'n_steps': 12288</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'gamma': 0.9591029149494671</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'gae_lambda': 0.9541845003001236</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'clip_range': 0.10331326443472709</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ent_coef': 0.02661587350926783}</t>
+  </si>
+  <si>
+    <t>{'reset_noise_scale': 0.09578929233536823</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'forward_reward_weight': 1.7429234815641454</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ctrl_cost_weight': 1.2489277534682572</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'healthy_reward': 2.465857784440316</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'contact_cost_weight': 4.3589765806323675e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'healthy_z_lower': 0.3413951260140689</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'healthy_z_upper': 1.3057167416301527</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'contact_force_min': -1.192846651406859</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'contact_force_max': 1.0724279378513066</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'learning_rate': 0.0008066765307245294</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'gamma': 0.956833700373414</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'gae_lambda': 0.9782417047710235</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'clip_range': 0.14429906555607105</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ent_coef': 0.02251015458483032}.</t>
+  </si>
+  <si>
+    <t>P_16</t>
+  </si>
+  <si>
+    <t>P_17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -689,6 +782,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -716,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -727,6 +826,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9067D9-17F2-1D45-A495-3CDCF8C57E4C}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1834,6 +1934,118 @@
         <v>200</v>
       </c>
     </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2740</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2805</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>